<commit_message>
new rules are working fine with new rules xlsx and new rules response
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D26A0C-946B-4221-B285-467AFE8A2805}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4164F710-96D3-4397-B066-917B8E7F1DA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -55,14 +55,14 @@
     <t>CONDITIONS</t>
   </si>
   <si>
-    <t>{
+    <t>[{
 	"message": "[LDAP: error code 49 - 80090308: LdapErr: DSID-0C09042F, comment: AcceptSecurityContext error, data 531, v2580 ]"
-}</t>
-  </si>
-  <si>
-    <t>{
+}]</t>
+  </si>
+  <si>
+    <t>[{
 	"message": "Security token is invalid. java.util.NoSuchElementException: No value present"
-}</t>
+}]</t>
   </si>
 </sst>
 </file>
@@ -417,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714F7F56-6336-4F26-AB0D-719E73D15D1F}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -464,7 +464,6 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="54.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
get all rules api
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4164F710-96D3-4397-B066-917B8E7F1DA1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD11BBF-5103-4068-91D4-BE4A7212FB77}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>RULE</t>
   </si>
@@ -42,14 +42,6 @@
   </si>
   <si>
     <t>R2</t>
-  </si>
-  <si>
-    <t>Solution1:
-1. Ask client for microsoft error debugging.</t>
-  </si>
-  <si>
-    <t>Solution2:
-1. Ask client for Security token .</t>
   </si>
   <si>
     <t>CONDITIONS</t>
@@ -63,6 +55,26 @@
     <t>[{
 	"message": "Security token is invalid. java.util.NoSuchElementException: No value present"
 }]</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Solution1: R1:
+1. Ask client for microsoft error debugging.</t>
+  </si>
+  <si>
+    <t>Solution2: R2: 
+1. Ask client for Security token .</t>
+  </si>
+  <si>
+    <t>[{
+	"message": "VALUEADDCO"
+}]</t>
+  </si>
+  <si>
+    <t>Solution2: R3:
+1. Problem is in VALUEADDCO, Ask client to change the value.</t>
   </si>
 </sst>
 </file>
@@ -417,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714F7F56-6336-4F26-AB0D-719E73D15D1F}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,7 +448,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -447,10 +459,10 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -458,11 +470,25 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>5</v>
-      </c>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
desc added in rul
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\IntellijIdeaProjects\LogAnalyzer\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD11BBF-5103-4068-91D4-BE4A7212FB77}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0882763-8843-4B34-8621-F058C5275505}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>RULE</t>
   </si>
@@ -75,6 +75,18 @@
   <si>
     <t>Solution2: R3:
 1. Problem is in VALUEADDCO, Ask client to change the value.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LDAP Configuration </t>
+  </si>
+  <si>
+    <t>Security Token Configuration Check</t>
+  </si>
+  <si>
+    <t>Value Addco Check</t>
   </si>
 </sst>
 </file>
@@ -429,66 +441,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714F7F56-6336-4F26-AB0D-719E73D15D1F}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="43.140625" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" customWidth="1"/>
-    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="1" max="2" width="14.85546875" customWidth="1"/>
+    <col min="3" max="3" width="43.140625" customWidth="1"/>
+    <col min="4" max="4" width="46.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="171.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Improved rules execution, added variables and regex successfully
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\My Downloads\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B359BE0D-D543-438E-8937-3A078B69CCDA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57434881-E8D0-47B2-879A-65E21BA32F4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -67,28 +67,6 @@
     <t>(
 (
 ( ( {
-	"message": "TOKEN: abc, TOKEN: def, TOKEN: ghi, REGEX:[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}, VAR: var1, REGEX:Bar[0-9]{2}-sector[0-9]{2}, VAR: var2 "
-} AND {
-	"message": "TOKEN:Messaging"
-} ) OR ( {
-	"message": "TOKEN:Messaging"
-} AND {
-	"message": "TOKEN:updates"
-}) )
-) AND
-{
-	"message": "TOKEN:DistributedMessaging"
-}
-)
-OR
-{
-	"message": "TOKEN:DistributedMessaging Watchdog - subscriber watchdog looking for updates"
-}</t>
-  </si>
-  <si>
-    <t>(
-(
-( ( {
 	"message": "TOKEN:DistributedMessaging"
 } AND {
 	"message": "TOKEN:Watchdog"
@@ -105,6 +83,28 @@
 OR
 {
 	"message": "TOKEN:DistributedMessaging Watchdog - subscriber watchdog looking for updates"
+}</t>
+  </si>
+  <si>
+    <t>(
+(
+( ( {
+	"message": "TOKEN: abc, TOKEN: def, TOKEN: ghi, REGEX:[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}, VAR: var1, REGEX:Bar[0-9]{2}-sector[0-9]{2}, VAR: var2 "
+} AND {
+	"message": "TOKEN:Messaging, VAR:{var2}"
+} ) OR ( {
+	"message": "TOKEN:Messaging, VAR:{var2}"
+} AND {
+	"message": "TOKEN:updates, VAR:{var2}"
+}) )
+) AND
+{
+	"message": "TOKEN:DistributedMessaging, VAR:{var2}"
+}
+)
+OR
+{
+	"message": "TOKEN:DistributedMessaging Watchdog - subscriber watchdog looking for updates, VAR:{var2}"
 }</t>
   </si>
 </sst>
@@ -463,7 +463,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,7 +497,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -511,7 +511,7 @@
         <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
BEFORE AFTER keywords added, converted into postfix also, need to write algorithm now to execute BEFORE AFTER
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\My Downloads\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D9F074-8BBE-4B64-AA01-C6AF7732A3C1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594A5430-A983-4716-B04A-A1926CE4BB31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -90,11 +90,11 @@
 (
 ( ( {
 	"message": "TOKEN: abc, TOKEN: def, TOKEN: ghi, REGEX:[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}, VAR: var1, REGEX:Bar[0-9]{2}-sector[0-9]{2}, VAR: var2 "
-} AND {
+} AND AFTER 00:00:00:980 {
 	"message": "TOKEN:Node down, VAR:{var1}"
 } ) OR ( {
 	"message": "TOKEN:Node down, VAR:{var1}"
-} AND {
+} AND BEFORE 00:00:00:876 {
 	"message": "TOKEN:Node down, VAR:{var1}"
 }) )
 ) AND
@@ -463,7 +463,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Rule Execution is working fine, Need to check if there are many patterns found and there are multiple values of var1 and need to replace each value every time we search for it,
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\My Downloads\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{594A5430-A983-4716-B04A-A1926CE4BB31}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06640FFD-04DF-4EA7-B662-ED605E8C32F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>RULE</t>
   </si>
@@ -90,7 +90,7 @@
 (
 ( ( {
 	"message": "TOKEN: abc, TOKEN: def, TOKEN: ghi, REGEX:[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}, VAR: var1, REGEX:Bar[0-9]{2}-sector[0-9]{2}, VAR: var2 "
-} AND AFTER 00:00:00:980 {
+} AND AFTER 00:00:00:100 {
 	"message": "TOKEN:Node down, VAR:{var1}"
 } ) OR ( {
 	"message": "TOKEN:Node down, VAR:{var1}"
@@ -106,6 +106,23 @@
 {
 	"message": "TOKEN:Node down, VAR:{var1}"
 }</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>Node Down</t>
+  </si>
+  <si>
+    <t>Solution3: R3:
+1. Node Down Errror.</t>
+  </si>
+  <si>
+    <t>( {
+	"message": "TOKEN: abc, TOKEN: def, TOKEN: ghi, REGEX:[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}, VAR: var1, REGEX:Bar[0-9]{2}-sector[0-9]{2}, VAR: var2 "
+} AND AFTER 00:00:00:100 {
+	"message": "TOKEN:Node down, VAR:{var1}"
+} )</t>
   </si>
 </sst>
 </file>
@@ -460,10 +477,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714F7F56-6336-4F26-AB0D-719E73D15D1F}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,6 +534,20 @@
         <v>9</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
XML reader attributes found
</commit_message>
<xml_diff>
--- a/src/main/resources/rules2.xlsx
+++ b/src/main/resources/rules2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gagan.gupta\My Downloads\logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06640FFD-04DF-4EA7-B662-ED605E8C32F3}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5914C00-3EDC-4B72-922F-F2A75324B0FB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{23E78A84-7340-4E68-AE3D-1D845B81F667}"/>
   </bookViews>
@@ -120,7 +120,7 @@
   <si>
     <t>( {
 	"message": "TOKEN: abc, TOKEN: def, TOKEN: ghi, REGEX:[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}-[0-9a-z]{4}, VAR: var1, REGEX:Bar[0-9]{2}-sector[0-9]{2}, VAR: var2 "
-} AND AFTER 00:00:00:100 {
+} AND AFTER 00:00:00:10 {
 	"message": "TOKEN:Node down, VAR:{var1}"
 } )</t>
   </si>
@@ -480,7 +480,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>